<commit_message>
vault backup: 2024-03-08 09:05:06
</commit_message>
<xml_diff>
--- a/projects/mrr-reporting/ops-activations-rollup-template.xlsx
+++ b/projects/mrr-reporting/ops-activations-rollup-template.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ian.wheeler\OneDrive - Meriplex Communications, Ltd\Documents\MERIPLEX\PROJECTS\Reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://meriplex-my.sharepoint.com/personal/ian_wheeler_meriplex_com/Documents/Documents/Obsidian/Meriplex/projects/mrr-reporting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C351078-E8F4-4AC4-8A54-3963080D8F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{6C351078-E8F4-4AC4-8A54-3963080D8F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C75D15F-7052-4C5F-9654-E1DA9ADA266C}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="570" windowWidth="14610" windowHeight="15585" xr2:uid="{ED36DC77-E424-4E7A-86BB-8127C1F608EE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{ED36DC77-E424-4E7A-86BB-8127C1F608EE}"/>
   </bookViews>
   <sheets>
     <sheet name="WoW" sheetId="1" r:id="rId1"/>
-    <sheet name="MoM" sheetId="2" r:id="rId2"/>
-    <sheet name="QoQ" sheetId="4" r:id="rId3"/>
-    <sheet name="Walk" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
+    <sheet name="MoM" sheetId="2" r:id="rId3"/>
+    <sheet name="QoQ" sheetId="4" r:id="rId4"/>
+    <sheet name="Walk" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="81">
   <si>
     <t>Meriplex Core WoW</t>
   </si>
@@ -245,6 +246,45 @@
   </si>
   <si>
     <t>when we buy and resell something,e.g., M365 liceses; we pay $10 per user/ and we charge $25 per user, e.g., Gross is $25, the net is $15</t>
+  </si>
+  <si>
+    <t>Block (NRR)</t>
+  </si>
+  <si>
+    <t>Block Recurring (MRR)</t>
+  </si>
+  <si>
+    <t>Refresh Rate:</t>
+  </si>
+  <si>
+    <t>Filters:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Projects </t>
+  </si>
+  <si>
+    <t>Opportunities Won</t>
+  </si>
+  <si>
+    <t>hrs remaining as a card with drill down</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> revenue remaining as a card with drill down</t>
+  </si>
+  <si>
+    <t>No filters</t>
+  </si>
+  <si>
+    <t>Once a Day (6AM CST)</t>
+  </si>
+  <si>
+    <t>Total Opps won without Project reference (as a card with drill down)</t>
+  </si>
+  <si>
+    <t>Total Number of Projects &gt; 60 Days old</t>
+  </si>
+  <si>
+    <t>Name: Backlog Report</t>
   </si>
 </sst>
 </file>
@@ -551,12 +591,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -578,9 +618,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -618,7 +658,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -724,7 +764,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -866,7 +906,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -876,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76FD83AC-1FAD-49FA-92B6-90DA619AF632}">
   <dimension ref="A1:U48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,7 +1093,7 @@
       </c>
     </row>
     <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="40" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="8"/>
@@ -1079,7 +1119,7 @@
       <c r="T9" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="U9" s="43" t="s">
+      <c r="U9" s="41" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1646,6 +1686,91 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{806DA1F5-CD8E-432B-B86B-1474465CAC8D}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F7422F-6383-44BC-910D-64131F852CFE}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1659,7 +1784,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45B65BFD-58E3-452C-9316-59F4DC0D608C}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1673,7 +1798,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26AA6B95-BEB9-4B9C-811D-C3C592E3D38D}">
   <dimension ref="A1:M21"/>
   <sheetViews>
@@ -1692,12 +1817,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
       <c r="E1" s="23"/>
       <c r="F1" s="23"/>
       <c r="G1" s="23"/>
@@ -1707,10 +1832,10 @@
       <c r="K1" s="23"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
       <c r="E2" s="23"/>
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
@@ -1720,8 +1845,8 @@
       <c r="K2" s="23"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="40"/>
-      <c r="B3" s="40"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="42"/>
       <c r="C3" s="23"/>
       <c r="D3" s="24" t="s">
         <v>42</v>
@@ -1963,10 +2088,10 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
       <c r="E16" s="23"/>
       <c r="F16" s="23"/>
       <c r="G16" s="23"/>
@@ -1991,10 +2116,10 @@
       <c r="K17" s="31"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
       <c r="E18" s="23"/>
       <c r="F18" s="23"/>
       <c r="G18" s="23"/>
@@ -2034,8 +2159,8 @@
       <c r="K20" s="33"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="40"/>
-      <c r="B21" s="40"/>
+      <c r="A21" s="42"/>
+      <c r="B21" s="42"/>
       <c r="C21" s="22"/>
       <c r="D21" s="34"/>
       <c r="E21" s="34"/>

</xml_diff>